<commit_message>
Added Example Data File
</commit_message>
<xml_diff>
--- a/Technical Design/Example Data.xlsx
+++ b/Technical Design/Example Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philip/Documents/SWE Project/Intro-to-Software-Engineering-Project/Technical Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A1EB1A1-3491-4042-8807-BF9369EB25C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF51BDF-1F4A-514C-8DC2-140848688867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B887F075-B753-A440-8F01-C7C9A9DFF519}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Users Entity</t>
   </si>
@@ -44,15 +44,6 @@
     <t>UserID PK</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>isAdmin</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -83,9 +74,6 @@
     <t>sWe.cCs_e</t>
   </si>
   <si>
-    <t>Products Entity</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -134,9 +122,6 @@
     <t>ShippingTypeId</t>
   </si>
   <si>
-    <t xml:space="preserve">ProductId PK </t>
-  </si>
-  <si>
     <t>ShippingTypeId PK</t>
   </si>
   <si>
@@ -164,9 +149,6 @@
     <t>UserId</t>
   </si>
   <si>
-    <t>ProducId</t>
-  </si>
-  <si>
     <t>SoldDate</t>
   </si>
   <si>
@@ -197,20 +179,80 @@
     <t>1348 20th Street NW, Rochester, MN, 55901</t>
   </si>
   <si>
-    <t>555-999-1688</t>
-  </si>
-  <si>
     <t>3847569322456020</t>
   </si>
   <si>
     <t>03/25</t>
+  </si>
+  <si>
+    <t>ShippingTypeCost</t>
+  </si>
+  <si>
+    <t>1100 S Marietta Parkway, Marietta, GA, 30060</t>
+  </si>
+  <si>
+    <t>555-678-9101</t>
+  </si>
+  <si>
+    <t>05/25</t>
+  </si>
+  <si>
+    <t>1000 Chastain Rd NW, Kennesaw, GA, 30144</t>
+  </si>
+  <si>
+    <t>555-999-4852</t>
+  </si>
+  <si>
+    <t>555-745-7545</t>
+  </si>
+  <si>
+    <t>8965215678541290</t>
+  </si>
+  <si>
+    <t>4512369547262450</t>
+  </si>
+  <si>
+    <t>04/24</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/starwars/images/7/7d/LukeROTJsaber-MR.jpg/revision/latest?cb=20100616172523</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/naruto-roleplay/images/8/84/Samehada.png/revision/latest?cb=20220531113104</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/4118OXbnIfL._AC_UF1000,1000_QL80_.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/f/f9/Master_Sword_Lead.png</t>
+  </si>
+  <si>
+    <t>https://i.etsystatic.com/31309176/r/il/d2d8a1/3470993913/il_570xN.3470993913_dzap.jpg</t>
+  </si>
+  <si>
+    <t>Inventory Entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InventoryId PK </t>
+  </si>
+  <si>
+    <t>InventoryId</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>IsAdmin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,6 +264,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,17 +294,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,22 +620,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C28C89-7224-2B4D-96C5-6C7C684E7F1A}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="70.1640625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="22.1640625" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -595,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -609,10 +664,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -623,10 +678,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -637,10 +692,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -651,10 +706,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -665,10 +720,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -676,24 +731,24 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -701,13 +756,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="D11" s="2">
         <v>15000</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -715,13 +773,16 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="D12" s="2">
         <v>30000</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -729,13 +790,16 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="2">
         <v>7000</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -743,13 +807,16 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="D14" s="2">
         <v>45000</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -757,116 +824,122 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="D15" s="2">
         <v>10000</v>
       </c>
       <c r="E15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="C18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="G24" t="s">
         <v>40</v>
       </c>
-      <c r="B24" t="s">
+      <c r="H24" t="s">
         <v>41</v>
       </c>
-      <c r="C24" t="s">
+      <c r="I24" t="s">
         <v>42</v>
       </c>
-      <c r="D24" t="s">
+      <c r="J24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" t="s">
+        <v>49</v>
+      </c>
+      <c r="M24" t="s">
         <v>43</v>
       </c>
-      <c r="E24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="N24" t="s">
         <v>45</v>
       </c>
-      <c r="G24" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" t="s">
-        <v>31</v>
-      </c>
-      <c r="K24" t="s">
-        <v>49</v>
-      </c>
-      <c r="L24" t="s">
-        <v>50</v>
-      </c>
-      <c r="M24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -875,35 +948,427 @@
         <v>45244</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="I25">
         <v>234</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="2">
+        <v>45000</v>
+      </c>
+      <c r="K25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>29</v>
+      </c>
+      <c r="M25" s="2">
+        <v>2700</v>
+      </c>
+      <c r="N25" s="2">
+        <v>47729</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3">
+        <v>45245</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26">
+        <v>762</v>
+      </c>
+      <c r="J26" s="2">
+        <v>10000</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>600</v>
+      </c>
+      <c r="N26" s="2">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45273</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27">
+        <v>842</v>
+      </c>
+      <c r="J27" s="2">
+        <v>15000</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>19</v>
+      </c>
+      <c r="M27">
+        <v>900</v>
+      </c>
+      <c r="N27" s="2">
+        <v>15919</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{8B18B7C3-714C-41D0-A557-51FE5B699303}"/>
+    <hyperlink ref="C12" r:id="rId2" xr:uid="{8A89A6AE-29F7-4906-BA27-59FF8D7109ED}"/>
+    <hyperlink ref="C13" r:id="rId3" xr:uid="{C57BB015-EA00-4E29-8FA5-7DA9D5E30A7A}"/>
+    <hyperlink ref="C14" r:id="rId4" xr:uid="{7848CC58-B53F-462B-B238-CADEE0E794A8}"/>
+    <hyperlink ref="C15" r:id="rId5" xr:uid="{3573420D-B633-4533-8C71-CB788E062331}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="888b9ef4-371e-4d81-bdd9-34172b121949" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FEAFD330E843124883D8F1143CB20504" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4867f3ed969d9f9c4e288d1a9aaf9cea">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="888b9ef4-371e-4d81-bdd9-34172b121949" xmlns:ns4="afaac706-6368-4a31-90da-43b31af501e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78e5a5756d085a6d16c44138e622f6df" ns3:_="" ns4:_="">
+    <xsd:import namespace="888b9ef4-371e-4d81-bdd9-34172b121949"/>
+    <xsd:import namespace="afaac706-6368-4a31-90da-43b31af501e1"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="888b9ef4-371e-4d81-bdd9-34172b121949" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="12" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="16" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="22" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="afaac706-6368-4a31-90da-43b31af501e1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="19" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0D5C41-5B96-49F8-ADC2-31C280FA6586}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="888b9ef4-371e-4d81-bdd9-34172b121949"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="afaac706-6368-4a31-90da-43b31af501e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C6BBF64-CBDA-445D-B725-6A30542707B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB042F98-ACCC-46CE-835B-CF1AC6B410C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="888b9ef4-371e-4d81-bdd9-34172b121949"/>
+    <ds:schemaRef ds:uri="afaac706-6368-4a31-90da-43b31af501e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>